<commit_message>
cleaned up pin map files
</commit_message>
<xml_diff>
--- a/DIYIOT - Board and Sensor Pin Map.xlsx
+++ b/DIYIOT - Board and Sensor Pin Map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37300" windowHeight="21960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DIYIOT - Board and Sensor Pin M" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="187">
   <si>
     <t>Board</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>KY-023 XY-axis joystick module</t>
-  </si>
-  <si>
-    <t>KY-024 Linear magnetic Hall sensors</t>
   </si>
   <si>
     <t>KY-025 Reed module</t>
@@ -589,7 +586,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -609,6 +606,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -662,12 +666,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1027,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P74"/>
+  <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1041,1462 +1046,1576 @@
     <col min="6" max="6" width="5.83203125" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" customWidth="1"/>
     <col min="8" max="8" width="5.33203125" customWidth="1"/>
+    <col min="14" max="14" width="3" customWidth="1"/>
+    <col min="15" max="15" width="33.33203125" customWidth="1"/>
     <col min="16" max="16" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" t="s">
         <v>108</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>109</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>110</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>111</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>112</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>113</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>114</v>
       </c>
-      <c r="L1" t="s">
-        <v>115</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="O1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>106</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" t="s">
+        <v>106</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" t="s">
+        <v>106</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" t="s">
+        <v>106</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" t="s">
+        <v>106</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" t="s">
+        <v>106</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" t="s">
+        <v>106</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" t="s">
+        <v>106</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" t="s">
+        <v>106</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" t="s">
+        <v>106</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12" t="s">
+        <v>106</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" t="s">
+        <v>106</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="B14" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" t="s">
         <v>116</v>
       </c>
-      <c r="F2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" t="s">
-        <v>107</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G3" t="s">
-        <v>107</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G4" t="s">
-        <v>107</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F5" t="s">
-        <v>106</v>
-      </c>
-      <c r="G5" t="s">
-        <v>107</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" t="s">
-        <v>107</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" t="s">
-        <v>107</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G8" t="s">
-        <v>107</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E9" t="s">
-        <v>116</v>
-      </c>
-      <c r="F9" t="s">
-        <v>106</v>
-      </c>
-      <c r="G9" t="s">
-        <v>107</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" t="s">
-        <v>116</v>
-      </c>
-      <c r="F10" t="s">
-        <v>106</v>
-      </c>
-      <c r="G10" t="s">
-        <v>107</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F11" t="s">
-        <v>106</v>
-      </c>
-      <c r="G11" t="s">
-        <v>107</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" t="s">
-        <v>101</v>
-      </c>
-      <c r="B12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F12" t="s">
-        <v>106</v>
-      </c>
-      <c r="G12" t="s">
-        <v>107</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" t="s">
-        <v>119</v>
-      </c>
-      <c r="F13" t="s">
-        <v>106</v>
-      </c>
-      <c r="G13" t="s">
-        <v>107</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="B14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C14" t="s">
-        <v>126</v>
-      </c>
-      <c r="E14" t="s">
-        <v>116</v>
-      </c>
-      <c r="F14" t="s">
-        <v>106</v>
-      </c>
-      <c r="G14" t="s">
-        <v>107</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="O15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
         <v>155</v>
       </c>
-      <c r="E15" t="s">
-        <v>107</v>
-      </c>
-      <c r="F15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G15" t="s">
-        <v>117</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" t="s">
-        <v>156</v>
-      </c>
       <c r="E16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G16" t="s">
-        <v>116</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>22</v>
+        <v>115</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
         <v>64</v>
       </c>
-      <c r="B17" t="s">
-        <v>65</v>
-      </c>
       <c r="C17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G17" t="s">
-        <v>116</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>24</v>
+        <v>115</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" t="s">
         <v>74</v>
       </c>
-      <c r="B18" t="s">
-        <v>75</v>
-      </c>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G18" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G19" t="s">
-        <v>116</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>27</v>
+        <v>115</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" t="s">
         <v>85</v>
       </c>
-      <c r="B20" t="s">
-        <v>86</v>
-      </c>
       <c r="C20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G20" t="s">
-        <v>116</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>28</v>
+        <v>115</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
         <v>37</v>
       </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
       <c r="C21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G21" t="s">
-        <v>116</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>29</v>
+        <v>115</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:16">
       <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
         <v>41</v>
       </c>
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
       <c r="C22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G22" t="s">
-        <v>116</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>30</v>
+        <v>115</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
         <v>47</v>
       </c>
-      <c r="B23" t="s">
-        <v>48</v>
-      </c>
       <c r="C23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G23" t="s">
-        <v>116</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>31</v>
+        <v>115</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
         <v>53</v>
       </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
       <c r="C24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G24" t="s">
-        <v>116</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>25</v>
+        <v>115</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
         <v>57</v>
       </c>
-      <c r="B25" t="s">
-        <v>58</v>
-      </c>
       <c r="C25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G25" t="s">
-        <v>107</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>26</v>
+        <v>106</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:16">
       <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" t="s">
         <v>89</v>
       </c>
-      <c r="B26" t="s">
-        <v>90</v>
-      </c>
       <c r="C26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G26" t="s">
-        <v>116</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>33</v>
+        <v>115</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:16">
       <c r="B27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G27" t="s">
-        <v>116</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="B28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G28" t="s">
-        <v>116</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>35</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:16">
       <c r="A29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" t="s">
         <v>99</v>
       </c>
-      <c r="B29" t="s">
-        <v>100</v>
-      </c>
       <c r="C29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J29" t="s">
-        <v>169</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>21</v>
+        <v>168</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:16">
       <c r="B30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c r="B31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:16">
       <c r="B32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:16">
       <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
         <v>66</v>
       </c>
-      <c r="B33" t="s">
-        <v>67</v>
-      </c>
       <c r="C33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E33" t="s">
+        <v>116</v>
+      </c>
+      <c r="F33" t="s">
         <v>117</v>
       </c>
-      <c r="F33" t="s">
-        <v>118</v>
-      </c>
       <c r="G33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J33" t="s">
-        <v>169</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>5</v>
+        <v>168</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:16">
       <c r="B34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G34" t="s">
+        <v>115</v>
+      </c>
+      <c r="H34" t="s">
         <v>116</v>
-      </c>
-      <c r="H34" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:16">
       <c r="B35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G35" t="s">
+        <v>115</v>
+      </c>
+      <c r="H35" t="s">
         <v>116</v>
-      </c>
-      <c r="H35" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:16">
       <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" t="s">
         <v>51</v>
       </c>
-      <c r="B36" t="s">
-        <v>52</v>
-      </c>
       <c r="C36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F36" t="s">
+        <v>128</v>
+      </c>
+      <c r="G36" t="s">
         <v>129</v>
       </c>
-      <c r="G36" t="s">
-        <v>130</v>
-      </c>
       <c r="H36" t="s">
-        <v>107</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>6</v>
+        <v>106</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:16">
       <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" t="s">
         <v>62</v>
       </c>
-      <c r="B37" t="s">
-        <v>63</v>
-      </c>
       <c r="C37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F37" t="s">
+        <v>128</v>
+      </c>
+      <c r="G37" t="s">
         <v>129</v>
       </c>
-      <c r="G37" t="s">
-        <v>130</v>
-      </c>
       <c r="H37" t="s">
-        <v>107</v>
-      </c>
-      <c r="P37" s="1" t="s">
-        <v>23</v>
+        <v>106</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:16">
       <c r="A38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" t="s">
         <v>72</v>
       </c>
-      <c r="B38" t="s">
-        <v>73</v>
-      </c>
       <c r="C38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G38" t="s">
-        <v>106</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>7</v>
+        <v>105</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" t="s">
         <v>78</v>
       </c>
-      <c r="B39" t="s">
-        <v>79</v>
-      </c>
       <c r="C39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J39" t="s">
-        <v>170</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>1</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:16">
       <c r="A40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" t="s">
         <v>82</v>
       </c>
-      <c r="B40" t="s">
-        <v>83</v>
-      </c>
       <c r="C40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J40" t="s">
-        <v>169</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>2</v>
+        <v>168</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:16">
       <c r="A41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" t="s">
         <v>95</v>
       </c>
-      <c r="B41" t="s">
-        <v>96</v>
-      </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J41" t="s">
-        <v>170</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>3</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:16">
       <c r="A42" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" t="s">
         <v>97</v>
       </c>
-      <c r="B42" t="s">
-        <v>98</v>
-      </c>
       <c r="C42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E42" t="s">
+        <v>116</v>
+      </c>
+      <c r="F42" t="s">
+        <v>106</v>
+      </c>
+      <c r="G42" t="s">
+        <v>105</v>
+      </c>
+      <c r="H42" t="s">
+        <v>124</v>
+      </c>
+      <c r="J42" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="P43" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="P44" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="P45" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="P46" s="1"/>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E42" t="s">
-        <v>117</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="D51" s="3"/>
+      <c r="E51" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+    </row>
+    <row r="54" spans="1:15">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="3"/>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E56" t="s">
         <v>107</v>
       </c>
-      <c r="G42" t="s">
-        <v>106</v>
-      </c>
-      <c r="H42" t="s">
-        <v>125</v>
-      </c>
-      <c r="J42" t="s">
-        <v>170</v>
-      </c>
-      <c r="P42" s="1" t="s">
+      <c r="F56" t="s">
+        <v>108</v>
+      </c>
+      <c r="G56" t="s">
+        <v>109</v>
+      </c>
+      <c r="H56" t="s">
+        <v>110</v>
+      </c>
+      <c r="I56" t="s">
+        <v>111</v>
+      </c>
+      <c r="J56" t="s">
+        <v>112</v>
+      </c>
+      <c r="K56" t="s">
+        <v>113</v>
+      </c>
+      <c r="L56" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" t="s">
+        <v>139</v>
+      </c>
+      <c r="B57">
+        <v>8</v>
+      </c>
+      <c r="E57">
+        <v>7</v>
+      </c>
+      <c r="F57">
+        <v>6</v>
+      </c>
+      <c r="G57">
+        <v>5</v>
+      </c>
+      <c r="H57">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:16">
-      <c r="A44" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16">
-      <c r="B45" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16">
-      <c r="B46" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16">
-      <c r="B47" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16">
-      <c r="B48" t="s">
-        <v>137</v>
-      </c>
-      <c r="C48" t="s">
-        <v>162</v>
-      </c>
-      <c r="E48" t="s">
-        <v>117</v>
-      </c>
-      <c r="F48" t="s">
-        <v>107</v>
-      </c>
-      <c r="G48" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49" t="s">
-        <v>103</v>
-      </c>
-      <c r="B49" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" t="s">
-        <v>183</v>
-      </c>
-      <c r="E49" t="s">
-        <v>107</v>
-      </c>
-      <c r="F49" t="s">
-        <v>106</v>
-      </c>
-      <c r="G49" t="s">
-        <v>120</v>
-      </c>
-      <c r="H49" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50" t="s">
-        <v>76</v>
-      </c>
-      <c r="B50" t="s">
-        <v>77</v>
-      </c>
-      <c r="E50" t="s">
-        <v>107</v>
-      </c>
-      <c r="F50" t="s">
-        <v>106</v>
-      </c>
-      <c r="G50" t="s">
-        <v>127</v>
-      </c>
-      <c r="H50" t="s">
-        <v>128</v>
-      </c>
-      <c r="I50" t="s">
-        <v>122</v>
-      </c>
-      <c r="K50" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="B51" t="s">
-        <v>149</v>
-      </c>
-      <c r="E51" t="s">
-        <v>106</v>
-      </c>
-      <c r="F51" t="s">
-        <v>116</v>
-      </c>
-      <c r="G51" t="s">
-        <v>117</v>
-      </c>
-      <c r="H51" t="s">
-        <v>107</v>
-      </c>
-      <c r="I51" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54" t="s">
-        <v>146</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E54" t="s">
-        <v>108</v>
-      </c>
-      <c r="F54" t="s">
-        <v>109</v>
-      </c>
-      <c r="G54" t="s">
-        <v>110</v>
-      </c>
-      <c r="H54" t="s">
-        <v>111</v>
-      </c>
-      <c r="I54" t="s">
-        <v>112</v>
-      </c>
-      <c r="J54" t="s">
-        <v>113</v>
-      </c>
-      <c r="K54" t="s">
-        <v>114</v>
-      </c>
-      <c r="L54" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13">
-      <c r="A55" t="s">
+      <c r="I57">
+        <v>3</v>
+      </c>
+      <c r="J57">
+        <v>2</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57" t="s">
+        <v>150</v>
+      </c>
+      <c r="M57" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58" t="s">
         <v>140</v>
-      </c>
-      <c r="B55">
-        <v>8</v>
-      </c>
-      <c r="E55">
-        <v>7</v>
-      </c>
-      <c r="F55">
-        <v>6</v>
-      </c>
-      <c r="G55">
-        <v>5</v>
-      </c>
-      <c r="H55">
-        <v>4</v>
-      </c>
-      <c r="I55">
-        <v>3</v>
-      </c>
-      <c r="J55">
-        <v>2</v>
-      </c>
-      <c r="K55">
-        <v>1</v>
-      </c>
-      <c r="L55" t="s">
-        <v>151</v>
-      </c>
-      <c r="M55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13">
-      <c r="A56" t="s">
-        <v>141</v>
-      </c>
-      <c r="B56">
-        <v>3</v>
-      </c>
-      <c r="E56" t="s">
-        <v>116</v>
-      </c>
-      <c r="F56" t="s">
-        <v>106</v>
-      </c>
-      <c r="G56" t="s">
-        <v>107</v>
-      </c>
-      <c r="M56" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13">
-      <c r="A57" t="s">
-        <v>142</v>
-      </c>
-      <c r="B57">
-        <v>3</v>
-      </c>
-      <c r="E57" t="s">
-        <v>107</v>
-      </c>
-      <c r="F57" t="s">
-        <v>106</v>
-      </c>
-      <c r="G57" t="s">
-        <v>117</v>
-      </c>
-      <c r="M57" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
-      <c r="A58" t="s">
-        <v>143</v>
       </c>
       <c r="B58">
         <v>3</v>
       </c>
       <c r="E58" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="F58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G58" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="M58" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B59">
         <v>3</v>
       </c>
       <c r="E59" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F59" t="s">
+        <v>105</v>
+      </c>
+      <c r="G59" t="s">
         <v>116</v>
       </c>
-      <c r="G59" t="s">
-        <v>106</v>
-      </c>
       <c r="M59" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B60">
         <v>3</v>
       </c>
       <c r="E60" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="F60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G60" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="M60" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61" t="s">
+        <v>143</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="E61" t="s">
+        <v>106</v>
+      </c>
+      <c r="F61" t="s">
+        <v>115</v>
+      </c>
+      <c r="G61" t="s">
+        <v>105</v>
+      </c>
+      <c r="M61" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
+      <c r="A62" t="s">
+        <v>144</v>
+      </c>
+      <c r="B62">
+        <v>3</v>
+      </c>
+      <c r="E62" t="s">
+        <v>116</v>
+      </c>
+      <c r="F62" t="s">
+        <v>105</v>
+      </c>
+      <c r="G62" t="s">
+        <v>106</v>
+      </c>
+      <c r="M62" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
+      <c r="A63" t="s">
+        <v>151</v>
+      </c>
+      <c r="B63">
+        <v>4</v>
+      </c>
+      <c r="E63" t="s">
+        <v>105</v>
+      </c>
+      <c r="F63" t="s">
+        <v>106</v>
+      </c>
+      <c r="G63" t="s">
+        <v>115</v>
+      </c>
+      <c r="H63" t="s">
+        <v>116</v>
+      </c>
+      <c r="M63" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
+      <c r="A64" t="s">
         <v>152</v>
-      </c>
-      <c r="B61">
-        <v>4</v>
-      </c>
-      <c r="E61" t="s">
-        <v>106</v>
-      </c>
-      <c r="F61" t="s">
-        <v>107</v>
-      </c>
-      <c r="G61" t="s">
-        <v>116</v>
-      </c>
-      <c r="H61" t="s">
-        <v>117</v>
-      </c>
-      <c r="M61" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="A62" t="s">
-        <v>153</v>
-      </c>
-      <c r="B62">
-        <v>4</v>
-      </c>
-      <c r="E62" t="s">
-        <v>126</v>
-      </c>
-      <c r="F62" t="s">
-        <v>107</v>
-      </c>
-      <c r="G62" t="s">
-        <v>124</v>
-      </c>
-      <c r="H62" t="s">
-        <v>107</v>
-      </c>
-      <c r="M62" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13">
-      <c r="A63" t="s">
-        <v>158</v>
-      </c>
-      <c r="B63">
-        <v>3</v>
-      </c>
-      <c r="E63" t="s">
-        <v>116</v>
-      </c>
-      <c r="F63" t="s">
-        <v>107</v>
-      </c>
-      <c r="G63" t="s">
-        <v>106</v>
-      </c>
-      <c r="M63" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
-      <c r="A64" t="s">
-        <v>160</v>
       </c>
       <c r="B64">
         <v>4</v>
       </c>
       <c r="E64" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="F64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G64" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="H64" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="M64" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:13">
       <c r="A65" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B65">
-        <v>4</v>
-      </c>
-      <c r="C65" t="s">
-        <v>168</v>
+        <v>3</v>
       </c>
       <c r="E65" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="F65" t="s">
         <v>106</v>
       </c>
       <c r="G65" t="s">
-        <v>166</v>
-      </c>
-      <c r="H65" t="s">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="M65" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:13">
       <c r="A66" t="s">
-        <v>174</v>
+        <v>159</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
       </c>
       <c r="E66" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G66" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="H66" t="s">
+        <v>124</v>
       </c>
       <c r="M66" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:13">
       <c r="A67" t="s">
-        <v>175</v>
+        <v>164</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>134</v>
+        <v>167</v>
+      </c>
+      <c r="E67" t="s">
+        <v>106</v>
+      </c>
+      <c r="F67" t="s">
+        <v>105</v>
+      </c>
+      <c r="G67" t="s">
+        <v>165</v>
+      </c>
+      <c r="H67" t="s">
+        <v>166</v>
+      </c>
+      <c r="M67" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:13">
       <c r="A68" t="s">
-        <v>176</v>
-      </c>
-      <c r="C68" t="s">
-        <v>179</v>
+        <v>173</v>
+      </c>
+      <c r="E68" t="s">
+        <v>116</v>
+      </c>
+      <c r="F68" t="s">
+        <v>106</v>
+      </c>
+      <c r="G68" t="s">
+        <v>105</v>
+      </c>
+      <c r="M68" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C69" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
+      <c r="A70" t="s">
+        <v>175</v>
+      </c>
+      <c r="C70" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="71" spans="1:13">
       <c r="A71" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C71" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13">
-      <c r="A72" t="s">
-        <v>181</v>
-      </c>
-      <c r="C72" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" t="s">
-        <v>185</v>
-      </c>
-      <c r="B73">
-        <v>3</v>
-      </c>
-      <c r="E73" t="s">
-        <v>106</v>
-      </c>
-      <c r="F73" t="s">
-        <v>116</v>
-      </c>
-      <c r="G73" t="s">
-        <v>107</v>
+        <v>179</v>
+      </c>
+      <c r="C73" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="74" spans="1:13">
       <c r="A74" t="s">
+        <v>180</v>
+      </c>
+      <c r="C74" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="A75" t="s">
+        <v>184</v>
+      </c>
+      <c r="B75">
+        <v>3</v>
+      </c>
+      <c r="E75" t="s">
+        <v>105</v>
+      </c>
+      <c r="F75" t="s">
+        <v>115</v>
+      </c>
+      <c r="G75" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
+      <c r="A76" t="s">
+        <v>185</v>
+      </c>
+      <c r="C76" t="s">
         <v>186</v>
-      </c>
-      <c r="C74" t="s">
-        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2504,40 +2623,39 @@
     <sortCondition ref="C2:C42"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="P39" r:id="rId1" tooltip="Arduino KY-001 Temperature sensor module"/>
-    <hyperlink ref="P40" r:id="rId2" tooltip="Arduino KY-002 Vibration switch module"/>
-    <hyperlink ref="P41" r:id="rId3" tooltip="Arduino KY-003 Hall magnetic sensor module"/>
-    <hyperlink ref="P42" r:id="rId4" tooltip="Arduino KY-004 Key switch module"/>
-    <hyperlink ref="P33" r:id="rId5" tooltip="Arduino KY-005 Infrared emission sensor module"/>
-    <hyperlink ref="P36" r:id="rId6" tooltip="Arduino KY-006 Small passive buzzer module"/>
-    <hyperlink ref="P38" r:id="rId7" tooltip="Arduino KY-008 Laser sensor module"/>
-    <hyperlink ref="P2" r:id="rId8" tooltip="Arduino KY-009 3-color full-color LED SMD modules"/>
-    <hyperlink ref="P3" r:id="rId9" tooltip="Arduino KY-010 Optical broken module"/>
-    <hyperlink ref="P4" r:id="rId10" tooltip="Arduino KY-011 2-color LED module"/>
-    <hyperlink ref="P5" r:id="rId11" tooltip="Arduino KY-012 Active buzzer module"/>
-    <hyperlink ref="P6" r:id="rId12" tooltip="Arduino KY-013 Temperature sensor module"/>
-    <hyperlink ref="P7" r:id="rId13" tooltip="Arduino KY-015 Temperature and humidity sensor module"/>
-    <hyperlink ref="P8" r:id="rId14" tooltip="Arduino KY-016 3-color LED module"/>
-    <hyperlink ref="P9" r:id="rId15" tooltip="Arduino KY-017 Mercury open optical module"/>
-    <hyperlink ref="P10" r:id="rId16" tooltip="Arduino KY-018 Photo resistor module"/>
-    <hyperlink ref="P11" r:id="rId17" tooltip="Arduino KY-019 5V relay module"/>
-    <hyperlink ref="P12" r:id="rId18" tooltip="Arduino KY-020 Tilt switch module"/>
-    <hyperlink ref="P13" r:id="rId19" tooltip="Arduino KY-021 Mini magnetic reed modules"/>
-    <hyperlink ref="P14" r:id="rId20" tooltip="Arduino KY-022 Infrared sensor receiver module"/>
-    <hyperlink ref="P29" r:id="rId21" tooltip="Arduino KY-023 XY-axis joystick module"/>
-    <hyperlink ref="P16" r:id="rId22" tooltip="Arduino KY-024 Linear magnetic Hall sensors"/>
-    <hyperlink ref="P37" r:id="rId23" tooltip="Arduino KY-025 Reed module"/>
-    <hyperlink ref="P17" r:id="rId24" tooltip="Arduino KY-026 Flame sensor module"/>
-    <hyperlink ref="P25" r:id="rId25" tooltip="Arduino KY-028 Temperature sensor module"/>
-    <hyperlink ref="P19" r:id="rId26" tooltip="Arduino KY-029 Yin Yi 2-color LED module 3MM"/>
-    <hyperlink ref="P20" r:id="rId27" tooltip="Arduino KY-031 Sensor module"/>
-    <hyperlink ref="P21" r:id="rId28" tooltip="Arduino KY-032 Obstacle avoidance sensor module"/>
-    <hyperlink ref="P22" r:id="rId29" tooltip="Arduino KY-033 Hunt sensor module"/>
-    <hyperlink ref="P23" r:id="rId30" tooltip="Arduino KY-034 Automatic flashing colorful LED module"/>
-    <hyperlink ref="P15" r:id="rId31" tooltip="Arduino KY-035 Class Bihor magnetic sensor"/>
-    <hyperlink ref="P26" r:id="rId32" tooltip="Arduino KY-038 Microphone sound sensor module"/>
-    <hyperlink ref="P27" r:id="rId33" tooltip="Arduino KY-039 Detect the heartbeat module"/>
-    <hyperlink ref="P28" r:id="rId34" tooltip="Arduino KY-040 Rotary encoder module"/>
+    <hyperlink ref="O21" r:id="rId1" tooltip="Arduino KY-001 Temperature sensor module"/>
+    <hyperlink ref="O2" r:id="rId2" tooltip="Arduino KY-002 Vibration switch module"/>
+    <hyperlink ref="O22" r:id="rId3" tooltip="Arduino KY-003 Hall magnetic sensor module"/>
+    <hyperlink ref="O3" r:id="rId4" tooltip="Arduino KY-004 Key switch module"/>
+    <hyperlink ref="O4" r:id="rId5" tooltip="Arduino KY-005 Infrared emission sensor module"/>
+    <hyperlink ref="O23" r:id="rId6" tooltip="Arduino KY-006 Small passive buzzer module"/>
+    <hyperlink ref="O5" r:id="rId7" tooltip="Arduino KY-008 Laser sensor module"/>
+    <hyperlink ref="O36" r:id="rId8" tooltip="Arduino KY-009 3-color full-color LED SMD modules"/>
+    <hyperlink ref="O24" r:id="rId9" tooltip="Arduino KY-010 Optical broken module"/>
+    <hyperlink ref="O20" r:id="rId10" tooltip="Arduino KY-011 2-color LED module"/>
+    <hyperlink ref="O25" r:id="rId11" tooltip="Arduino KY-012 Active buzzer module"/>
+    <hyperlink ref="O6" r:id="rId12" tooltip="Arduino KY-013 Temperature sensor module"/>
+    <hyperlink ref="O7" r:id="rId13" tooltip="Arduino KY-015 Temperature and humidity sensor module"/>
+    <hyperlink ref="O37" r:id="rId14" tooltip="Arduino KY-016 3-color LED module"/>
+    <hyperlink ref="O17" r:id="rId15" tooltip="Arduino KY-017 Mercury open optical module"/>
+    <hyperlink ref="O33" r:id="rId16" tooltip="Arduino KY-018 Photo resistor module"/>
+    <hyperlink ref="O8" r:id="rId17" tooltip="Arduino KY-019 5V relay module"/>
+    <hyperlink ref="O9" r:id="rId18" tooltip="Arduino KY-020 Tilt switch module"/>
+    <hyperlink ref="O38" r:id="rId19" tooltip="Arduino KY-021 Mini magnetic reed modules"/>
+    <hyperlink ref="O18" r:id="rId20" tooltip="Arduino KY-022 Infrared sensor receiver module"/>
+    <hyperlink ref="P44" r:id="rId21" tooltip="Arduino KY-023 XY-axis joystick module"/>
+    <hyperlink ref="O10" r:id="rId22" tooltip="Arduino KY-025 Reed module"/>
+    <hyperlink ref="O40" r:id="rId23" tooltip="Arduino KY-026 Flame sensor module"/>
+    <hyperlink ref="O19" r:id="rId24" tooltip="Arduino KY-028 Temperature sensor module"/>
+    <hyperlink ref="O16" r:id="rId25" tooltip="Arduino KY-029 Yin Yi 2-color LED module 3MM"/>
+    <hyperlink ref="O13" r:id="rId26" tooltip="Arduino KY-031 Sensor module"/>
+    <hyperlink ref="P43" r:id="rId27" tooltip="Arduino KY-032 Obstacle avoidance sensor module"/>
+    <hyperlink ref="O26" r:id="rId28" tooltip="Arduino KY-033 Hunt sensor module"/>
+    <hyperlink ref="O11" r:id="rId29" tooltip="Arduino KY-034 Automatic flashing colorful LED module"/>
+    <hyperlink ref="O15" r:id="rId30" tooltip="Arduino KY-035 Class Bihor magnetic sensor"/>
+    <hyperlink ref="O29" r:id="rId31" tooltip="Arduino KY-038 Microphone sound sensor module"/>
+    <hyperlink ref="O12" r:id="rId32" tooltip="Arduino KY-039 Detect the heartbeat module"/>
+    <hyperlink ref="O52" r:id="rId33" tooltip="Arduino KY-040 Rotary encoder module"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>